<commit_message>
fix bridge melee and LZ archer
</commit_message>
<xml_diff>
--- a/contents/battle_1/battle_1.xlsx
+++ b/contents/battle_1/battle_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imanol-KS53\Documents\Imanol\Github_projects\InteractiveBook\contents\battle_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC3721C-5F9E-474A-826A-BF8A42C6374D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035E6881-385D-46F1-9465-0914801955EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="45">
   <si>
     <t>x</t>
   </si>
@@ -559,7 +559,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,6 +855,9 @@
       <c r="E14" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="G14" s="10" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -953,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>36</v>
@@ -970,10 +973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A63502-AF7A-4054-B79C-125248EE72B4}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1006,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
@@ -1016,7 +1019,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
@@ -1029,7 +1032,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -1047,6 +1050,7 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -1061,10 +1065,11 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>9</v>
+      <c r="A7" t="s">
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
@@ -1086,56 +1091,12 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="D13">
+      <c r="D9">
         <v>-1</v>
       </c>
     </row>
@@ -1150,7 +1111,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix deployment by difficulty
</commit_message>
<xml_diff>
--- a/contents/battle_1/battle_1.xlsx
+++ b/contents/battle_1/battle_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imanol-KS53\Documents\Imanol\Github_projects\InteractiveBook\contents\battle_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035E6881-385D-46F1-9465-0914801955EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91350435-B059-4663-95CF-A5A3B7477A0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -558,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -1110,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35488FFD-9895-4BA3-BA35-EBF213FD10A0}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,7 +1630,7 @@
         <v>2</v>
       </c>
       <c r="J16">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
offset and scale nodes
</commit_message>
<xml_diff>
--- a/contents/battle_1/battle_1.xlsx
+++ b/contents/battle_1/battle_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imanol-KS53\Documents\Imanol\Github_projects\InteractiveBook\contents\battle_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9FDB38-AEAD-4A09-960C-5058C31C56DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EBD9CE-005C-4BE4-BDAB-E7B63EAF1884}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,10 +968,10 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>16</v>
+        <v>15.5</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1131,7 +1131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35488FFD-9895-4BA3-BA35-EBF213FD10A0}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
define interactions parameters in excel
</commit_message>
<xml_diff>
--- a/contents/battle_1/battle_1.xlsx
+++ b/contents/battle_1/battle_1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imanol-KS53\Documents\Imanol\Github_projects\InteractiveBook\contents\battle_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EBD9CE-005C-4BE4-BDAB-E7B63EAF1884}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86651A5D-E0EE-4C39-9B5B-57D45557B0E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
     <sheet name="interactions" sheetId="2" r:id="rId2"/>
     <sheet name="units" sheetId="3" r:id="rId3"/>
+    <sheet name="parameters" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
   <si>
     <t>x</t>
   </si>
@@ -168,6 +169,36 @@
   </si>
   <si>
     <t>attack_range</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>melee_distance</t>
+  </si>
+  <si>
+    <t>melee_height_difference_threshold</t>
+  </si>
+  <si>
+    <t>archer_distance</t>
+  </si>
+  <si>
+    <t>archer_distance_height_gain</t>
+  </si>
+  <si>
+    <t>siege_distance</t>
+  </si>
+  <si>
+    <t>siege_distance_height_gain</t>
+  </si>
+  <si>
+    <t>flier_distance</t>
+  </si>
+  <si>
+    <t>flier_distance_height_gain</t>
   </si>
 </sst>
 </file>
@@ -576,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1812,4 +1843,95 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1402C5AC-6BA8-4199-9EF0-F087CEA6081F}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add monster and cavalry classes
</commit_message>
<xml_diff>
--- a/contents/battle_1/battle_1.xlsx
+++ b/contents/battle_1/battle_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imanol-KS53\Documents\Imanol\Github_projects\InteractiveBook\contents\battle_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86651A5D-E0EE-4C39-9B5B-57D45557B0E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BA0693-EEB6-41F3-835A-CE5D862DF0D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="60">
   <si>
     <t>x</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>flier_distance_height_gain</t>
+  </si>
+  <si>
+    <t>cavalry_distance</t>
+  </si>
+  <si>
+    <t>cavalry_height_difference_threshold</t>
+  </si>
+  <si>
+    <t>cavalry</t>
   </si>
 </sst>
 </file>
@@ -1022,15 +1031,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A63502-AF7A-4054-B79C-125248EE72B4}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -1047,10 +1056,13 @@
         <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>24</v>
       </c>
@@ -1062,8 +1074,11 @@
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>25</v>
       </c>
@@ -1075,8 +1090,11 @@
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>26</v>
       </c>
@@ -1088,8 +1106,11 @@
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>40</v>
       </c>
@@ -1103,8 +1124,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>41</v>
       </c>
@@ -1118,8 +1142,11 @@
         <v>1</v>
       </c>
       <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1130,7 +1157,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
@@ -1141,7 +1168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1847,10 +1874,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1402C5AC-6BA8-4199-9EF0-F087CEA6081F}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1917,17 +1944,33 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>56</v>
       </c>
-      <c r="B9">
+      <c r="B11">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>